<commit_message>
Pluto Foreign Currency,Checks & Drafts Updated Code
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSheet/Data.xlsx
+++ b/src/test/resources/DataSheet/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5685" windowWidth="11520" windowHeight="1170" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="5685" windowWidth="11520" windowHeight="1170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderDetails" sheetId="5" r:id="rId1"/>
@@ -425,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10163" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10257" uniqueCount="1207">
   <si>
     <t>AutomationID</t>
   </si>
@@ -3943,18 +3943,12 @@
     <t>Test Test</t>
   </si>
   <si>
-    <t>AutoTest</t>
-  </si>
-  <si>
     <t>testuser</t>
   </si>
   <si>
     <t>Next Day - Home Branch</t>
   </si>
   <si>
-    <t>Foreign Currency#Australian Dollar#1000#5,10#100,50</t>
-  </si>
-  <si>
     <t>AutoChelsea1</t>
   </si>
   <si>
@@ -3995,6 +3989,63 @@
   </si>
   <si>
     <t>ShippingCharge</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Canadian Dollar#1000#5,10#100,50</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>HomeTelephoneNo</t>
+  </si>
+  <si>
+    <t>Travelex</t>
+  </si>
+  <si>
+    <t>Paradigam</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>United States Of America - USA</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>AwayBranchLocation</t>
+  </si>
+  <si>
+    <t>AlternateTeller</t>
+  </si>
+  <si>
+    <t>AlternateTellerName</t>
+  </si>
+  <si>
+    <t>CollectionCheck</t>
+  </si>
+  <si>
+    <t>ConfigAdditionalInfo</t>
+  </si>
+  <si>
+    <t>AutoChelsea3</t>
+  </si>
+  <si>
+    <t>Drafts#Australian Dollar#1000#BenificiaryName,Address1,Address2,Mumbai,UNITED STATES OF AMERICA,California,517214,DraftComment</t>
+  </si>
+  <si>
+    <t>AutoChelsea4</t>
+  </si>
+  <si>
+    <t>Checks#Canadian Dollar#1000</t>
   </si>
 </sst>
 </file>
@@ -19492,7 +19543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AH3" sqref="AH3"/>
     </sheetView>
@@ -19629,10 +19680,10 @@
         <v>87</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>105</v>
@@ -37085,10 +37136,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37103,19 +37154,26 @@
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="131.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="17.42578125" customWidth="1"/>
+    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -37123,7 +37181,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
@@ -37150,61 +37208,84 @@
         <v>1159</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>1161</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>1160</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>1161</v>
-      </c>
       <c r="P1" s="6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>1190</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>1198</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>1202</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>1200</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>1162</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>1165</v>
+      </c>
+      <c r="AD1" s="6" t="s">
         <v>1163</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>1164</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>1165</v>
-      </c>
-      <c r="U1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>1166</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>1167</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>1176</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D2" s="55" t="s">
         <v>1178</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>1180</v>
-      </c>
       <c r="E2" s="26" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>1168</v>
@@ -37222,57 +37303,87 @@
         <v>43</v>
       </c>
       <c r="K2" s="55" t="s">
+        <v>1183</v>
+      </c>
+      <c r="L2" s="26" t="s">
         <v>1185</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="26" t="s">
-        <v>1187</v>
-      </c>
       <c r="P2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="55" t="s">
+        <v>1199</v>
+      </c>
+      <c r="Z2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="26" t="s">
         <v>1171</v>
       </c>
-      <c r="Q2" s="55" t="s">
+      <c r="AB2" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="AC2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AE2" s="26" t="s">
         <v>1172</v>
       </c>
-      <c r="S2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>1173</v>
-      </c>
-      <c r="V2" s="57" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF2" s="57" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>1177</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>1179</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>1183</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>1180</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>1181</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>43</v>
@@ -37287,43 +37398,269 @@
         <v>11</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="K3" s="55" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>43</v>
+        <v>1188</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>1175</v>
+        <v>42</v>
       </c>
       <c r="P3" s="26" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>1194</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>1195</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>1196</v>
+      </c>
+      <c r="T3" s="55" t="s">
+        <v>1197</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V3" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="W3" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>1199</v>
+      </c>
+      <c r="Z3" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="26" t="s">
         <v>1171</v>
       </c>
-      <c r="Q3" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="26" t="s">
+      <c r="AB3" s="56" t="s">
+        <v>557</v>
+      </c>
+      <c r="AC3" s="56" t="s">
+        <v>557</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AE3" s="26" t="s">
         <v>1172</v>
       </c>
-      <c r="S3" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="56" t="s">
+      <c r="AF3" s="57" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>1173</v>
+      </c>
+      <c r="K4" s="55" t="s">
+        <v>1183</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>1204</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>1194</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>1195</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>1196</v>
+      </c>
+      <c r="T4" s="55" t="s">
+        <v>1197</v>
+      </c>
+      <c r="U4" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="U3" s="26" t="s">
-        <v>1173</v>
-      </c>
-      <c r="V3" s="57" t="s">
-        <v>1186</v>
+      <c r="W4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y4" s="55" t="s">
+        <v>1199</v>
+      </c>
+      <c r="Z4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AB4" s="56" t="s">
+        <v>557</v>
+      </c>
+      <c r="AC4" s="56" t="s">
+        <v>557</v>
+      </c>
+      <c r="AD4" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AE4" s="26" t="s">
+        <v>1172</v>
+      </c>
+      <c r="AF4" s="57" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>1183</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>1206</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="W5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y5" s="55" t="s">
+        <v>1199</v>
+      </c>
+      <c r="Z5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AB5" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="AC5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD5" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AE5" s="26" t="s">
+        <v>1172</v>
+      </c>
+      <c r="AF5" s="57" t="s">
+        <v>1184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 'Additional Info' column in data sheet for louisville partner
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSheet/Data.xlsx
+++ b/src/test/resources/DataSheet/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5685" windowWidth="11520" windowHeight="1170" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="5745" windowWidth="11520" windowHeight="1170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderDetails" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -43,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -58,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -67,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -82,7 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -91,7 +91,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -106,7 +106,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -115,7 +115,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -154,7 +154,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -163,7 +163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -202,7 +202,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -211,7 +211,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -226,7 +226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -235,7 +235,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -274,7 +274,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Surve, Pravin:</t>
         </r>
@@ -283,7 +283,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 INV</t>
@@ -424,8 +424,70 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Surve, Pravin</author>
+  </authors>
+  <commentList>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Travelex Louisville
+Format:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Address 1#Address 2#Address 3#City#State#Telephone#ZipCode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Format:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 = today
+1 = tomorrow
+and so on.
+Max is 8</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10257" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10889" uniqueCount="1284">
   <si>
     <t>AutomationID</t>
   </si>
@@ -3940,27 +4002,12 @@
     <t>Account Holder</t>
   </si>
   <si>
-    <t>Test Test</t>
-  </si>
-  <si>
     <t>testuser</t>
   </si>
   <si>
     <t>Next Day - Home Branch</t>
   </si>
   <si>
-    <t>AutoChelsea1</t>
-  </si>
-  <si>
-    <t>AutoChelsea2</t>
-  </si>
-  <si>
-    <t>Pluto purchase order</t>
-  </si>
-  <si>
-    <t>Pluto Sale order</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -3979,12 +4026,6 @@
     <t>29668</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Foreign Currency#Australian Dollar#1000#NA#NA|Foreign Currency#Canadian Dollar#1000#NA#NA|Foreign Currency#Euro#1000#NA#NA</t>
-  </si>
-  <si>
     <t>ServiceCharge</t>
   </si>
   <si>
@@ -4036,23 +4077,275 @@
     <t>ConfigAdditionalInfo</t>
   </si>
   <si>
-    <t>AutoChelsea3</t>
-  </si>
-  <si>
-    <t>Drafts#Australian Dollar#1000#BenificiaryName,Address1,Address2,Mumbai,UNITED STATES OF AMERICA,California,517214,DraftComment</t>
-  </si>
-  <si>
-    <t>AutoChelsea4</t>
-  </si>
-  <si>
-    <t>Checks#Canadian Dollar#1000</t>
+    <t>AutoChelsea_2</t>
+  </si>
+  <si>
+    <t>Purchase | Checks | Single |</t>
+  </si>
+  <si>
+    <t>Customer Type 1</t>
+  </si>
+  <si>
+    <t>AutoChelsea_3</t>
+  </si>
+  <si>
+    <t>29669</t>
+  </si>
+  <si>
+    <t>AutoChelsea_4</t>
+  </si>
+  <si>
+    <t>Purchase | FC+Checks | Mixed |</t>
+  </si>
+  <si>
+    <t>Non-Account Holder</t>
+  </si>
+  <si>
+    <t>29670</t>
+  </si>
+  <si>
+    <t>AutoChelsea_5</t>
+  </si>
+  <si>
+    <t>Purchase | FC | Single |</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>29671</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Canadian Dollar#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_6</t>
+  </si>
+  <si>
+    <t>Purchase | FC | Multi |</t>
+  </si>
+  <si>
+    <t>Citigold</t>
+  </si>
+  <si>
+    <t>29672</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Neth. Antilles Guilder#1000#NA#NA|Foreign Currency#Aruba Florin#1000#NA#NA|Foreign Currency#Barbados Dollar#1000#NA#NA|Foreign Currency#Bulgarian Lev#1000#NA#NA|Foreign Currency#Bahraini Dinar#1000#NA#NA|Foreign Currency#Bermuda Dollar#1000#NA#NA|Foreign Currency#Brunei Dollar#1000#NA#NA|Foreign Currency#Bolivian Boliviano#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_7</t>
+  </si>
+  <si>
+    <t>Private Banking</t>
+  </si>
+  <si>
+    <t>29673</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Brazilian Real#1000#NA#NA|Foreign Currency#Belize Dollar#1000#NA#NA|Foreign Currency#Canadian Dollar#1000#NA#NA|Foreign Currency#Swiss Franc#1000#NA#NA|Foreign Currency#Chilean Peso#1000#NA#NA|Foreign Currency#Chinese Renminbi#1000#NA#NA\Foreign Currency#Colombian Peso#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_8</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>29674</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Costa Rica Colon#1000#NA#NA|Foreign Currency#Czech Koruna#1000#NA#NA|Foreign Currency#Danish Krone#1000#NA#NA|Foreign Currency#Dominican Peso#1000#NA#NA|Foreign Currency#Euro#1000#NA#NA\Foreign Currency#Fiji Dollar#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_9</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>29675</t>
+  </si>
+  <si>
+    <t>AutoChelsea_10</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>29676</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Hungarian Forint#1000#NA#NA|Foreign Currency#Indonesian Rupiah#1000#NA#NA|Foreign Currency#Israeli Shekel#1000#NA#NA|Foreign Currency#Indian Rupee#1000#NA#NA|Foreign Currency#Iceland Krona#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_11</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>29677</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Jamaican Dollar#1000#NA#NA|Foreign Currency#Jordanian Dinar#1000#NA#NA|Foreign Currency#Japanese Yen#1000#NA#NA|Foreign Currency#Kenyan Shilling#1000#NA#NA|Foreign Currency#Korean Won#1000#NA#NA|Foreign Currency#Kuwaiti Dinar#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_12</t>
+  </si>
+  <si>
+    <t>CitiBusiness</t>
+  </si>
+  <si>
+    <t>29678</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Cayman Islands Dollar#1000#NA#NA|Foreign Currency#Sri Lanka Rupee#1000#NA#NA|Foreign Currency#Moroccan Dirham#1000#NA#NA|Foreign Currency#Mauritius Rupee#1000#NA#NA|Foreign Currency#Mexican Nuevo Peso#1000#NA#NA</t>
+  </si>
+  <si>
+    <t>Test Comments</t>
+  </si>
+  <si>
+    <t>Checks#Japanese Yen#2#NA#NA|Checks#Japanese Yen#2#NA#NA</t>
+  </si>
+  <si>
+    <t>Checks#British Pound#100#NA#NA</t>
+  </si>
+  <si>
+    <t>Foreign Currency#UAE Dirham#10#NA#NA|Checks#Euro#2#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_01</t>
+  </si>
+  <si>
+    <t>AutoChelsea_02</t>
+  </si>
+  <si>
+    <t>AutoChelsea_03</t>
+  </si>
+  <si>
+    <t>AutoChelsea_04</t>
+  </si>
+  <si>
+    <t>AutoChelsea_05</t>
+  </si>
+  <si>
+    <t>AutoChelsea_06</t>
+  </si>
+  <si>
+    <t>AutoChelsea_07</t>
+  </si>
+  <si>
+    <t>AutoChelsea_08</t>
+  </si>
+  <si>
+    <t>AutoChelsea_09</t>
+  </si>
+  <si>
+    <t>TRAVELEX LOUISVILLE</t>
+  </si>
+  <si>
+    <t>Purchase | Checks | Multi | Same CCY |</t>
+  </si>
+  <si>
+    <t>Sale | FC+Drafts | Mixed | Home Branch | Denom |</t>
+  </si>
+  <si>
+    <t>Sale | Drafts | Multi | Same CCY | Away Branch |</t>
+  </si>
+  <si>
+    <t>Sale | FC | Single | Home Delivery |</t>
+  </si>
+  <si>
+    <t>Sale | FC | Multi |</t>
+  </si>
+  <si>
+    <t>Next Day - Away Branch</t>
+  </si>
+  <si>
+    <t>Next Day - Home Delivery</t>
+  </si>
+  <si>
+    <t>Priority - Away Branch</t>
+  </si>
+  <si>
+    <t>Priority - Home Branch</t>
+  </si>
+  <si>
+    <t>Priority - Home Delivery</t>
+  </si>
+  <si>
+    <t>Secure - Away Branch</t>
+  </si>
+  <si>
+    <t>Secure - Home Branch</t>
+  </si>
+  <si>
+    <t>Secure - Home Delivery</t>
+  </si>
+  <si>
+    <t>29679</t>
+  </si>
+  <si>
+    <t>29680</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Canadian Dollar#1000#5,10#100,50|Drafts#Australian Dollar#1000#BenificiaryName,Address1,Address2,Mumbai,UNITED STATES OF AMERICA,California,517214,DraftComment</t>
+  </si>
+  <si>
+    <t>Drafts#Australian Dollar#1000#BenificiaryName,Address1,Address2,Mumbai,UNITED STATES OF AMERICA,California,517214,DraftComment|Drafts#Australian Dollar#1000#BenificiaryName,Address1,Address2,Mumbai,UNITED STATES OF AMERICA,California,517214,DraftComment</t>
+  </si>
+  <si>
+    <t>Foreign Currency#UAE Dirham#700#1,1,2,5,10,20#200,100,50,20,10,5 |Foreign Currency#Neth. Antilles Guilder#400#1,2,4,10#100,50,25,10|Foreign Currency#Argentine Peso#900#1,2,5,10,20#500,50,20,10,5</t>
+  </si>
+  <si>
+    <t>Foreign Currency#British Pound#10#NA#NA|Foreign Currency#Gibraltar Pound#10#NA#NA|Foreign Currency#Hong Kong Dollar#10#NA#NA|Foreign Currency#Honduras Lempira#10#NA#NA|Foreign Currency#Croatian Kuna#10#NA#NA</t>
+  </si>
+  <si>
+    <t>AutoChelsea_1</t>
+  </si>
+  <si>
+    <t>AdditionalInfo</t>
+  </si>
+  <si>
+    <t>Purchase | FC+Checks | Mixed |TRAVELEX LOUISVILLE</t>
+  </si>
+  <si>
+    <t>Address1#Address2#Address3#Albany#New York#123654789#12206</t>
+  </si>
+  <si>
+    <t>AutoChelsea_010</t>
+  </si>
+  <si>
+    <t>AutoChelsea_011</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Aruba Florin#500#10,4,2,2#10,25,50,100|Foreign Currency#Barbados Dollar#600#50,20,10,5,2,1#2,5,10,20,50,100|Foreign Currency#Bulgarian Lev#400#10,5,2,1#10,20,50,100</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Bahraini Dinar#500#100,20,10,10#1,5,10,20|Foreign Currency#Bermuda Dollar#500#50,20,10,5,2#2,5,10,20,50|Foreign Currency#Brazilian Real#300#5,4#20,50</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Canadian Dollar#500#20,10,5,2,1#5,10,20,50,100|Foreign Currency#Swiss Franc#500#10,5,2,2#10,20,50,100|Foreign Currency#Chilean Peso#18000#1,1,1,1#1000,2000,5000,10000</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Chinese Renminbi#500#5#100|Foreign Currency#Colombian Peso#80000#1,1,1#10000,20000,50000|Foreign Currency#Costa Rica Colon#38000#1,1,1,1,1#1000,2000,5000,10000,20000</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Czech Koruna#8800#1,1,1,1,1,1#100,200,500,1000,2000,5000|Foreign Currency#Dominican Peso#3900#2,1,1,1,1,1#50,100,200,500,1000,2000|Foreign Currency#Euro#1200#20,10,5,2,1,1,1#5,10,20,50,100,200,500</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Fiji Dollar#400#10,5,2,1#10,20,50,100|Foreign Currency#British Pound#500#20,10,5,4#5,10,20,50|Foreign Currency#Guatemala Quetzal#500#5,2,1,1#20,50,100,200</t>
+  </si>
+  <si>
+    <t>Foreign Currency#Croatian Kuna#300#1,1#100,200|Foreign Currency#Hungarian Forint#38000#1,1,1,1,1#1000,2000,5000,10000,20000|Foreign Currency#Hong Kong Dollar#900#10,5,2,1,1#10,20,50,100,50|</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4107,17 +4400,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="14">
@@ -4264,7 +4551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4326,11 +4613,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19680,10 +19971,10 @@
         <v>87</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>1186</v>
+        <v>1179</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>1187</v>
+        <v>1180</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>105</v>
@@ -30910,8 +31201,8 @@
       <c r="AD123" s="43"/>
       <c r="AE123" s="43"/>
       <c r="AF123" s="43"/>
-      <c r="AG123" s="58"/>
-      <c r="AH123" s="58"/>
+      <c r="AG123" s="57"/>
+      <c r="AH123" s="57"/>
     </row>
     <row r="124" spans="1:34" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="19" t="s">
@@ -31462,8 +31753,8 @@
       <c r="AD129" s="43"/>
       <c r="AE129" s="43"/>
       <c r="AF129" s="43"/>
-      <c r="AG129" s="59"/>
-      <c r="AH129" s="59"/>
+      <c r="AG129" s="58"/>
+      <c r="AH129" s="58"/>
     </row>
     <row r="130" spans="1:34" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="22" t="s">
@@ -37135,24 +37426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="131.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -37162,18 +37453,19 @@
     <col min="19" max="19" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="17.42578125" customWidth="1"/>
-    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="17.42578125" customWidth="1"/>
+    <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -37181,7 +37473,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
@@ -37220,451 +37512,2389 @@
         <v>18</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>1189</v>
+        <v>1182</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>35</v>
       </c>
       <c r="U1" s="6" t="s">
+        <v>1185</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>1272</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>1195</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>1193</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>1162</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>1165</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>1166</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="60" t="s">
+        <v>1178</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>1240</v>
+      </c>
+      <c r="M2" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC2" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD2" s="61" t="s">
+        <v>557</v>
+      </c>
+      <c r="AE2" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF2" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="60" t="s">
+        <v>1200</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>1239</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X3" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC3" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE3" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="60" t="s">
+        <v>1204</v>
+      </c>
+      <c r="L4" s="59" t="s">
+        <v>1241</v>
+      </c>
+      <c r="M4" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC4" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE4" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF4" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="60" t="s">
+        <v>1208</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>1209</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W5" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG5" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>1212</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>1213</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M6" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X6" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG6" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="60" t="s">
+        <v>1217</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>1218</v>
+      </c>
+      <c r="M7" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X7" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG7" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="59" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="60" t="s">
+        <v>1221</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>1222</v>
+      </c>
+      <c r="M8" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X8" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y8" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE8" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG8" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>1225</v>
+      </c>
+      <c r="L9" s="59" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M9" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W9" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X9" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y9" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG9" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>1228</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>1229</v>
+      </c>
+      <c r="M10" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W10" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X10" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y10" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE10" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF10" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG10" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="60" t="s">
+        <v>1232</v>
+      </c>
+      <c r="L11" s="59" t="s">
+        <v>1233</v>
+      </c>
+      <c r="M11" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W11" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X11" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y11" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF11" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG11" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>1236</v>
+      </c>
+      <c r="L12" s="59" t="s">
+        <v>1237</v>
+      </c>
+      <c r="M12" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V12" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W12" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X12" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y12" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE12" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF12" s="59" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG12" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G13" s="59" t="s">
+        <v>1251</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="59" t="s">
+        <v>1241</v>
+      </c>
+      <c r="M13" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="P13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="V13" s="26" t="s">
+        <v>1274</v>
+      </c>
+      <c r="W13" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X13" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y13" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB13" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC13" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG13" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="62" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>1172</v>
+      </c>
+      <c r="K14" s="55" t="s">
+        <v>1265</v>
+      </c>
+      <c r="L14" s="59" t="s">
+        <v>1267</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="R14" s="26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S14" s="26" t="s">
+        <v>1189</v>
+      </c>
+      <c r="T14" s="55" t="s">
+        <v>1190</v>
+      </c>
+      <c r="U14" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W14" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X14" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y14" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z14" s="55" t="s">
         <v>1192</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>1164</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>1198</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>1202</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA14" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB14" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC14" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD14" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE14" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF14" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG14" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="62" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K15" s="55" t="s">
+        <v>1266</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>1268</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q15" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="R15" s="26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S15" s="26" t="s">
+        <v>1189</v>
+      </c>
+      <c r="T15" s="55" t="s">
+        <v>1190</v>
+      </c>
+      <c r="U15" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V15" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W15" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X15" s="55" t="s">
+        <v>1265</v>
+      </c>
+      <c r="Y15" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z15" s="55" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AA15" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB15" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC15" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD15" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE15" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF15" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG15" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="62" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>1258</v>
+      </c>
+      <c r="K16" s="55" t="s">
+        <v>1178</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>1181</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q16" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="R16" s="26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S16" s="26" t="s">
+        <v>1189</v>
+      </c>
+      <c r="T16" s="55" t="s">
+        <v>1190</v>
+      </c>
+      <c r="U16" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W16" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X16" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y16" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z16" s="55" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AA16" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB16" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC16" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD16" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE16" s="26" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AF16" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG16" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" s="62" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>1259</v>
+      </c>
+      <c r="K17" s="55" t="s">
         <v>1200</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>1201</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>1162</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>1165</v>
-      </c>
-      <c r="AD1" s="6" t="s">
+      <c r="L17" s="26" t="s">
+        <v>1269</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W17" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X17" s="55" t="s">
+        <v>1265</v>
+      </c>
+      <c r="Y17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC17" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD17" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF17" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG17" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>1212</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>1260</v>
+      </c>
+      <c r="K18" s="55" t="s">
+        <v>1204</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>1277</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W18" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC18" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD18" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF18" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG18" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K19" s="55" t="s">
+        <v>1208</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>1278</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q19" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="R19" s="26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S19" s="26" t="s">
+        <v>1189</v>
+      </c>
+      <c r="T19" s="55" t="s">
+        <v>1190</v>
+      </c>
+      <c r="U19" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W19" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X19" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y19" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z19" s="55" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AA19" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB19" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC19" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD19" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE19" s="26" t="s">
         <v>1163</v>
       </c>
-      <c r="AE1" s="6" t="s">
-        <v>1166</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="AF19" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG19" s="26" t="s">
         <v>1174</v>
       </c>
-      <c r="B2" s="26" t="s">
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" s="62" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>1176</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>1180</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>1168</v>
-      </c>
-      <c r="G2" s="26" t="s">
+      <c r="D20" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>1169</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>1170</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="55" t="s">
-        <v>1183</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>1185</v>
-      </c>
-      <c r="M2" s="26" t="s">
+      <c r="H20" s="26" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>1262</v>
+      </c>
+      <c r="K20" s="55" t="s">
+        <v>1213</v>
+      </c>
+      <c r="L20" s="26" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N20" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O20" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="55" t="s">
+      <c r="P20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T20" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U20" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W20" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="W2" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="55" t="s">
-        <v>1199</v>
-      </c>
-      <c r="Z2" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="26" t="s">
+      <c r="X20" s="55" t="s">
+        <v>1265</v>
+      </c>
+      <c r="Y20" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z20" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA20" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC20" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD20" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF20" s="26" t="s">
         <v>1171</v>
       </c>
-      <c r="AB2" s="55" t="s">
+      <c r="AG20" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="62" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B21" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>1263</v>
+      </c>
+      <c r="K21" s="60" t="s">
+        <v>1217</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>1280</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W21" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="AC2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD2" s="26" t="s">
+      <c r="X21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA21" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC21" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD21" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF21" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG21" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B22" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>1264</v>
+      </c>
+      <c r="K22" s="60" t="s">
+        <v>1221</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>1281</v>
+      </c>
+      <c r="M22" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="26" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q22" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="R22" s="26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="S22" s="26" t="s">
+        <v>1189</v>
+      </c>
+      <c r="T22" s="55" t="s">
+        <v>1190</v>
+      </c>
+      <c r="U22" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="V22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W22" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X22" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y22" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z22" s="55" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AA22" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB22" s="26" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AC22" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD22" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE22" s="26" t="s">
         <v>1163</v>
       </c>
-      <c r="AE2" s="26" t="s">
+      <c r="AF22" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG22" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" s="62" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B23" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="26" t="s">
         <v>1172</v>
       </c>
-      <c r="AF2" s="57" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>1175</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>1181</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="26" t="s">
+      <c r="K23" s="60" t="s">
+        <v>1225</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>1282</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W23" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="X23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC23" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD23" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF23" s="26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG23" s="26" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" s="62" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B24" s="59" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="26" t="s">
         <v>1169</v>
       </c>
-      <c r="H3" s="26" t="s">
-        <v>1170</v>
-      </c>
-      <c r="I3" s="26" t="s">
+      <c r="H24" s="26" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I24" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K3" s="55" t="s">
-        <v>1183</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>1188</v>
-      </c>
-      <c r="M3" s="26" t="s">
+      <c r="J24" s="26" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K24" s="60" t="s">
+        <v>1228</v>
+      </c>
+      <c r="L24" s="26" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M24" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N24" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O24" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="26" t="s">
-        <v>1193</v>
-      </c>
-      <c r="Q3" s="26" t="s">
-        <v>1194</v>
-      </c>
-      <c r="R3" s="26" t="s">
-        <v>1195</v>
-      </c>
-      <c r="S3" s="26" t="s">
-        <v>1196</v>
-      </c>
-      <c r="T3" s="55" t="s">
-        <v>1197</v>
-      </c>
-      <c r="U3" s="55" t="s">
-        <v>211</v>
-      </c>
-      <c r="V3" s="55" t="s">
+      <c r="P24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="U24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="V24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W24" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="W3" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y3" s="55" t="s">
-        <v>1199</v>
-      </c>
-      <c r="Z3" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" s="26" t="s">
+      <c r="X24" s="55" t="s">
+        <v>1265</v>
+      </c>
+      <c r="Y24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC24" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD24" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF24" s="26" t="s">
         <v>1171</v>
       </c>
-      <c r="AB3" s="56" t="s">
-        <v>557</v>
-      </c>
-      <c r="AC3" s="56" t="s">
-        <v>557</v>
-      </c>
-      <c r="AD3" s="26" t="s">
-        <v>1163</v>
-      </c>
-      <c r="AE3" s="26" t="s">
-        <v>1172</v>
-      </c>
-      <c r="AF3" s="57" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>1181</v>
-      </c>
-      <c r="D4" s="55" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>1169</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>1170</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K4" s="55" t="s">
-        <v>1183</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>1204</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>1193</v>
-      </c>
-      <c r="Q4" s="26" t="s">
-        <v>1194</v>
-      </c>
-      <c r="R4" s="26" t="s">
-        <v>1195</v>
-      </c>
-      <c r="S4" s="26" t="s">
-        <v>1196</v>
-      </c>
-      <c r="T4" s="55" t="s">
-        <v>1197</v>
-      </c>
-      <c r="U4" s="55" t="s">
-        <v>211</v>
-      </c>
-      <c r="V4" s="55" t="s">
-        <v>557</v>
-      </c>
-      <c r="W4" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y4" s="55" t="s">
-        <v>1199</v>
-      </c>
-      <c r="Z4" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA4" s="26" t="s">
-        <v>1171</v>
-      </c>
-      <c r="AB4" s="56" t="s">
-        <v>557</v>
-      </c>
-      <c r="AC4" s="56" t="s">
-        <v>557</v>
-      </c>
-      <c r="AD4" s="26" t="s">
-        <v>1163</v>
-      </c>
-      <c r="AE4" s="26" t="s">
-        <v>1172</v>
-      </c>
-      <c r="AF4" s="57" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>1176</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>1180</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>1168</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>1169</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>1170</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="55" t="s">
-        <v>1183</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>1206</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="R5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="T5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="V5" s="55" t="s">
-        <v>557</v>
-      </c>
-      <c r="W5" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" s="55" t="s">
-        <v>1199</v>
-      </c>
-      <c r="Z5" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA5" s="26" t="s">
-        <v>1171</v>
-      </c>
-      <c r="AB5" s="55" t="s">
-        <v>557</v>
-      </c>
-      <c r="AC5" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD5" s="26" t="s">
-        <v>1163</v>
-      </c>
-      <c r="AE5" s="26" t="s">
-        <v>1172</v>
-      </c>
-      <c r="AF5" s="57" t="s">
-        <v>1184</v>
+      <c r="AG24" s="26" t="s">
+        <v>1174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="AC2:AC4 K8:K12 K14:K24" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>